<commit_message>
Trying to get old code at least compile
</commit_message>
<xml_diff>
--- a/VNC Phidgets.xlsx
+++ b/VNC Phidgets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNC\Git\chrhodes\Phidgets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VNC\Git\chrhodes\Phidgets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D859A075-C0E5-496F-8A05-1D28CE357236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82745CDD-D951-454E-B1D7-7CAE8A6D74EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37250" windowHeight="21820" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Phidgets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -151,15 +151,25 @@
   </si>
   <si>
     <t>Rotation Sensor</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,18 +196,141 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -213,17 +346,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0">
-  <autoFilter ref="A4:E29" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:F29" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A4:F29" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D27">
     <sortCondition ref="A4:A27"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B5EDBEA5-DAE1-4F94-8C58-2EE5E26802CA}" name="Model"/>
-    <tableColumn id="2" xr3:uid="{1F2EF091-5960-4E10-8E8D-AE4CA65F357E}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{E1D52329-E985-4A59-BBA2-B2E125BF30E8}" name="Count"/>
-    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="0"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B5EDBEA5-DAE1-4F94-8C58-2EE5E26802CA}" name="Model" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1F2EF091-5960-4E10-8E8D-AE4CA65F357E}" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E1D52329-E985-4A59-BBA2-B2E125BF30E8}" name="Count" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1B0DEB78-7126-4930-B005-957E9180DAF1}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -526,313 +660,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00DB4F1-23DB-43B6-AF53-1598330C1B83}">
-  <dimension ref="A4:E29"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A4:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1328125" customWidth="1"/>
-    <col min="3" max="3" width="98.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="77.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>1012</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6">
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
         <v>1018</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7">
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>1056</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8">
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>1061</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9">
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>1062</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10">
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>1063</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11">
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>1064</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12">
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
         <v>1070</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13">
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>1072</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14">
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>1101</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>1102</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16">
+    <row r="16" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>1103</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17">
+    <row r="17" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>1104</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18">
+    <row r="18" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>1106</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19">
+    <row r="19" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>1108</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20">
+    <row r="20" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>1109</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21">
+    <row r="21" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>1110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22">
+    <row r="22" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>1111</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23">
+      <c r="E22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>1112</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24">
+    <row r="24" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
         <v>1113</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25">
+    <row r="25" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>1124</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26">
+    <row r="26" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>1127</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27">
+    <row r="27" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
         <v>1128</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28">
+      <c r="E27" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>3004</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29">
+    <row r="29" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
         <v>3051</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Well it compiles.  Now to try to understand what I was thinking over 10 years ago
</commit_message>
<xml_diff>
--- a/VNC Phidgets.xlsx
+++ b/VNC Phidgets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNC\Git\chrhodes\Phidgets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNC\git\chrhodes\Phidgets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D859A075-C0E5-496F-8A05-1D28CE357236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F6F944-A956-4293-BCCB-DD99E77173A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Phidgets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Model</t>
   </si>
@@ -151,16 +151,43 @@
   </si>
   <si>
     <t>Rotation Sensor</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>psbc1, 192.168.150.1</t>
+  </si>
+  <si>
+    <t>psbc21, 192.168.150.21</t>
+  </si>
+  <si>
+    <t>Serial #</t>
+  </si>
+  <si>
+    <t>Name, IP</t>
+  </si>
+  <si>
+    <t>psbc22, 192.168.150.22</t>
+  </si>
+  <si>
+    <t>psbc23, 192.168.150.23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,16 +213,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -213,17 +249,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0">
-  <autoFilter ref="A4:E29" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D27">
-    <sortCondition ref="A4:A27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:H31" totalsRowShown="0">
+  <autoFilter ref="A4:H31" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F29">
+    <sortCondition ref="A4:A29"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B5EDBEA5-DAE1-4F94-8C58-2EE5E26802CA}" name="Model"/>
     <tableColumn id="2" xr3:uid="{1F2EF091-5960-4E10-8E8D-AE4CA65F357E}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{23589240-397B-4E7D-8C8C-0C344DCF8B91}" name="Name, IP"/>
+    <tableColumn id="7" xr3:uid="{0388D911-9D48-4A55-AE07-48345C836D7E}" name="Serial #"/>
+    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{E1D52329-E985-4A59-BBA2-B2E125BF30E8}" name="Count"/>
-    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{E3DF68C1-F6AE-4B5A-8447-D920DAFFA772}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -526,21 +565,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00DB4F1-23DB-43B6-AF53-1598330C1B83}">
-  <dimension ref="A4:E29"/>
+  <dimension ref="A4:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1328125" customWidth="1"/>
-    <col min="3" max="3" width="98.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.08984375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -548,114 +589,123 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1012</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1018</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1056</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1061</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1062</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1063</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1064</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1070</v>
       </c>
@@ -663,13 +713,16 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1072</v>
       </c>
@@ -677,159 +730,206 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>48284</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
+        <v>1072</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>48301</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1072</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>251831</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>1101</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15">
+      <c r="G16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>1102</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>1103</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>1104</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>1106</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>1108</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>1109</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>1110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>1111</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23">
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>1112</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>1113</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>1124</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>1127</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>1128</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28">
+      <c r="G29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>3004</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>3051</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Update R/O fields in Attach
</commit_message>
<xml_diff>
--- a/VNC Phidgets.xlsx
+++ b/VNC Phidgets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNC\git\chrhodes\Phidgets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93999751-A7D1-4B75-B6AB-A64A6F564F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4FA9BD-450A-44D9-90D3-AF9DD6E8E1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31610" yWindow="1170" windowWidth="28440" windowHeight="18660" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
+    <workbookView xWindow="610" yWindow="2950" windowWidth="28800" windowHeight="15450" xr2:uid="{DDC81552-0E26-46A6-9AF2-B2F0938C3EFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Phidgets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>Model</t>
   </si>
@@ -172,13 +172,89 @@
   </si>
   <si>
     <t>psbc11, 192.168.150.1,5001</t>
+  </si>
+  <si>
+    <t>Illuminance (lux) = Voltage * 200</t>
+  </si>
+  <si>
+    <t>Discontinued</t>
+  </si>
+  <si>
+    <r>
+      <t>Temperature (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) = (VoltageRatio * 222.2) - 61.111</t>
+    </r>
+  </si>
+  <si>
+    <t>3521_0</t>
+  </si>
+  <si>
+    <t>3520_0</t>
+  </si>
+  <si>
+    <t>3522_0</t>
+  </si>
+  <si>
+    <t>Using reflected IR light, measure the distance of an opaque object 20-150cm away.</t>
+  </si>
+  <si>
+    <t>Using reflected IR light, measure the distance of an opaque object 4-30cm away.</t>
+  </si>
+  <si>
+    <t>Using reflected IR light, measure the distance of an opaque object 10-80cm away.</t>
+  </si>
+  <si>
+    <t>Sharp Distance Sensor (4-30cm) 2D120X</t>
+  </si>
+  <si>
+    <t>Sharp Distance Sensor (20-150cm) 2Y0A02</t>
+  </si>
+  <si>
+    <t>Sharp Distance Sensor (10-80cm) 2Y0A21</t>
+  </si>
+  <si>
+    <t>Distance (cm) = 2.076/(VoltageRatio - 0.011) Valid 0.08-0.53</t>
+  </si>
+  <si>
+    <t>Distance (cm) = 4.8/(VoltageRatio - 0.02) Valid 0.08-0.53</t>
+  </si>
+  <si>
+    <t>Distance (cm) = 9.462/(VoltageRatio - 0.01692) Valid 0.08-0.49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +267,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,11 +313,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -248,20 +343,122 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="&#10;\text{Illuminance (lux)} = \text{Voltage} \times 200&#10;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866F0879-2BDD-6D69-B35A-7F99A918838A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12261850" y="5340350"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="&#10;\text{Temperature (}^\circ \text{C)} = \text{(VoltageRatio} \times \text{222.2) - 61.111}&#10;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C311D3C2-3377-FF58-6BE2-671632DDE65F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11709400" y="5524500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:H31" totalsRowShown="0">
-  <autoFilter ref="A4:H31" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F29">
-    <sortCondition ref="A4:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}" name="Table1" displayName="Table1" ref="A4:I34" totalsRowShown="0">
+  <autoFilter ref="A4:I34" xr:uid="{3006E699-0B16-4E2D-A1B8-BFD01F7B1D7C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:I34">
+    <sortCondition ref="A4:A34"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B5EDBEA5-DAE1-4F94-8C58-2EE5E26802CA}" name="Model"/>
     <tableColumn id="2" xr3:uid="{1F2EF091-5960-4E10-8E8D-AE4CA65F357E}" name="Name"/>
+    <tableColumn id="9" xr3:uid="{63016717-9F32-4C07-B1D3-C2E7A03DB635}" name="Discontinued" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{23589240-397B-4E7D-8C8C-0C344DCF8B91}" name="Name, IP,Port"/>
     <tableColumn id="7" xr3:uid="{0388D911-9D48-4A55-AE07-48345C836D7E}" name="Serial #"/>
-    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{89BE91BB-B0F2-42E7-8966-7E0076CEC336}" name="Description" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{E1D52329-E985-4A59-BBA2-B2E125BF30E8}" name="Count"/>
-    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{70A8E98B-4CF9-41DD-A215-CAB80A92C2C8}" name="Printed Manual" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{E3DF68C1-F6AE-4B5A-8447-D920DAFFA772}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -565,377 +762,448 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00DB4F1-23DB-43B6-AF53-1598330C1B83}">
-  <dimension ref="A4:H31"/>
+  <dimension ref="A4:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" customWidth="1"/>
-    <col min="3" max="3" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.08984375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="52.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1012</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1018</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1056</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1061</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1062</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1063</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1064</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1070</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>46049</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1072</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>48284</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1072</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>45</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>48301</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1072</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>251831</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1101</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1102</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1103</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1104</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1106</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1108</v>
       </c>
       <c r="B21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1109</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1110</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1111</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1112</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1113</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1124</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1127</v>
       </c>
       <c r="B28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1128</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3004</v>
       </c>
       <c r="B30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3051</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>